<commit_message>
Alterei alguns DSS que achava que estavam mal
</commit_message>
<xml_diff>
--- a/Modelos UML/Descrição UseCases/CarroPronto.xlsx
+++ b/Modelos UML/Descrição UseCases/CarroPronto.xlsx
@@ -72,9 +72,6 @@
     <t>Alternativa [ID Inválido] (passo 5)</t>
   </si>
   <si>
-    <t>6. Adicionar carro à lista de carros produzidos</t>
-  </si>
-  <si>
     <t>5. Valida ID do carro</t>
   </si>
   <si>
@@ -88,6 +85,9 @@
   </si>
   <si>
     <t>7. Informa que operação foi realizada</t>
+  </si>
+  <si>
+    <t>6. Remove carro da lista de produção</t>
   </si>
 </sst>
 </file>
@@ -621,10 +621,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:D16"/>
+  <dimension ref="B1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -650,7 +650,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D3" s="14"/>
     </row>
@@ -715,52 +715,57 @@
       <c r="B11" s="12"/>
       <c r="C11" s="5"/>
       <c r="D11" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="12"/>
       <c r="C12" s="5"/>
       <c r="D12" s="1" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B13" s="12"/>
       <c r="C13" s="5"/>
       <c r="D13" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="12"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="1"/>
+    </row>
+    <row r="15" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="4"/>
-      <c r="D14" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="12"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="1" t="s">
+      <c r="C15" s="4"/>
+      <c r="D15" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="16" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="12"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="3"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B17" s="12"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="B15:B17"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C5:D5"/>
-    <mergeCell ref="B6:B13"/>
+    <mergeCell ref="B6:B14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fiz um bocado do relatório
</commit_message>
<xml_diff>
--- a/Modelos UML/Descrição UseCases/CarroPronto.xlsx
+++ b/Modelos UML/Descrição UseCases/CarroPronto.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pmcca\Documents\3º Ano\DSS\Trabalho\DSS\DSS\Modelos UML\Descrição UseCases\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luis\Documents\Luís\3º ano\1º Semestre\DSS\Trabalho\DSS\Modelos UML\Descrição UseCases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2D103C1-EC9C-4C0A-ABBC-AD6F3DC7E03F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="75" yWindow="465" windowWidth="25440" windowHeight="14715" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="75" yWindow="465" windowWidth="25440" windowHeight="14715"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -91,7 +90,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -618,11 +617,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>